<commit_message>
Fix gni_index position in output and remove duplicate country code
</commit_message>
<xml_diff>
--- a/output/clean_data.xlsx
+++ b/output/clean_data.xlsx
@@ -14,65 +14,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
-  <si>
-    <t>Country Code</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+  <si>
+    <t>country_index</t>
+  </si>
+  <si>
+    <t>Hult_Team_Regions</t>
+  </si>
+  <si>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>income_group</t>
+  </si>
+  <si>
+    <t>access_to_electricity_pop</t>
+  </si>
+  <si>
+    <t>access_to_electricity_rural</t>
+  </si>
+  <si>
+    <t>access_to_electricity_urban</t>
+  </si>
+  <si>
+    <t>CO2_emissions_per_capita)</t>
+  </si>
+  <si>
+    <t>compulsory_edu_yrs</t>
+  </si>
+  <si>
+    <t>pct_female_employment</t>
+  </si>
+  <si>
+    <t>pct_male_employment</t>
+  </si>
+  <si>
+    <t>pct_agriculture_employment</t>
+  </si>
+  <si>
+    <t>pct_industry_employment</t>
+  </si>
+  <si>
+    <t>pct_services_employment</t>
+  </si>
+  <si>
+    <t>exports_pct_gdp</t>
+  </si>
+  <si>
+    <t>fdi_pct_gdp</t>
   </si>
   <si>
     <t>gni_index</t>
   </si>
   <si>
-    <t>country_index</t>
-  </si>
-  <si>
-    <t>Hult_Team_Regions</t>
-  </si>
-  <si>
-    <t>country_name</t>
-  </si>
-  <si>
-    <t>country_code</t>
-  </si>
-  <si>
-    <t>income_group</t>
-  </si>
-  <si>
-    <t>access_to_electricity_pop</t>
-  </si>
-  <si>
-    <t>access_to_electricity_rural</t>
-  </si>
-  <si>
-    <t>access_to_electricity_urban</t>
-  </si>
-  <si>
-    <t>CO2_emissions_per_capita)</t>
-  </si>
-  <si>
-    <t>compulsory_edu_yrs</t>
-  </si>
-  <si>
-    <t>pct_female_employment</t>
-  </si>
-  <si>
-    <t>pct_male_employment</t>
-  </si>
-  <si>
-    <t>pct_agriculture_employment</t>
-  </si>
-  <si>
-    <t>pct_industry_employment</t>
-  </si>
-  <si>
-    <t>pct_services_employment</t>
-  </si>
-  <si>
-    <t>exports_pct_gdp</t>
-  </si>
-  <si>
-    <t>fdi_pct_gdp</t>
-  </si>
-  <si>
     <t>gdp_usd</t>
   </si>
   <si>
@@ -190,6 +187,51 @@
     <t>m_urban_population_growth_pct</t>
   </si>
   <si>
+    <t>Central Africa 1</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo, Dem. Rep.</t>
+  </si>
+  <si>
+    <t>Congo, Rep.</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
     <t>BDI</t>
   </si>
   <si>
@@ -230,51 +272,6 @@
   </si>
   <si>
     <t>UGA</t>
-  </si>
-  <si>
-    <t>Central Africa 1</t>
-  </si>
-  <si>
-    <t>Burundi</t>
-  </si>
-  <si>
-    <t>Cabo Verde</t>
-  </si>
-  <si>
-    <t>Comoros</t>
-  </si>
-  <si>
-    <t>Congo, Dem. Rep.</t>
-  </si>
-  <si>
-    <t>Congo, Rep.</t>
-  </si>
-  <si>
-    <t>Cote d'Ivoire</t>
-  </si>
-  <si>
-    <t>Equatorial Guinea</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t>Uganda</t>
   </si>
   <si>
     <t>Low income</t>
@@ -641,13 +638,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG15"/>
+  <dimension ref="A1:BF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:59">
+    <row r="1" spans="1:58">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,464 +816,455 @@
       <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:58">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:59">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2">
-        <v>290</v>
-      </c>
-      <c r="D2">
-        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>52.1</v>
+      </c>
+      <c r="J2">
+        <v>0.044485376</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>12.70699978</v>
+      </c>
+      <c r="M2">
+        <v>3.730000019</v>
+      </c>
+      <c r="N2">
+        <v>91.10299683</v>
+      </c>
+      <c r="O2">
+        <v>2.549000025</v>
+      </c>
+      <c r="P2">
+        <v>6.34800005</v>
+      </c>
+      <c r="Q2">
+        <v>7.76818252</v>
+      </c>
+      <c r="R2">
+        <v>2.642421428</v>
+      </c>
+      <c r="S2">
+        <v>290</v>
+      </c>
+      <c r="T2">
+        <v>3093647227</v>
+      </c>
+      <c r="U2">
+        <v>4.660918184</v>
+      </c>
+      <c r="V2">
+        <v>0.04</v>
+      </c>
+      <c r="W2">
+        <v>1.38</v>
+      </c>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Y2">
+        <v>61.56972885</v>
+      </c>
+      <c r="Z2">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="AA2">
+        <v>47.08506861</v>
+      </c>
+      <c r="AB2">
+        <v>30.5</v>
+      </c>
+      <c r="AC2">
+        <v>17.9</v>
+      </c>
+      <c r="AD2">
+        <v>1.570000052</v>
+      </c>
+      <c r="AE2">
+        <v>11.761</v>
+      </c>
+      <c r="AF2">
+        <v>5.480228006</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>1</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>52.1</v>
-      </c>
-      <c r="L2">
-        <v>0.044485376</v>
-      </c>
-      <c r="M2">
-        <v>6</v>
-      </c>
-      <c r="N2">
-        <v>12.70699978</v>
-      </c>
-      <c r="O2">
-        <v>3.730000019</v>
-      </c>
-      <c r="P2">
-        <v>91.10299683</v>
-      </c>
-      <c r="Q2">
-        <v>2.549000025</v>
-      </c>
-      <c r="R2">
-        <v>6.34800005</v>
-      </c>
-      <c r="S2">
-        <v>7.76818252</v>
-      </c>
-      <c r="T2">
-        <v>2.642421428</v>
-      </c>
-      <c r="U2">
-        <v>3093647227</v>
-      </c>
-      <c r="V2">
-        <v>4.660918184</v>
-      </c>
-      <c r="W2">
-        <v>0.04</v>
-      </c>
-      <c r="X2">
-        <v>1.38</v>
-      </c>
-      <c r="Y2">
-        <v>4</v>
-      </c>
-      <c r="Z2">
-        <v>61.56972885</v>
-      </c>
-      <c r="AA2">
-        <v>77.90000000000001</v>
-      </c>
-      <c r="AB2">
-        <v>47.08506861</v>
-      </c>
-      <c r="AC2">
-        <v>30.5</v>
-      </c>
-      <c r="AD2">
-        <v>17.9</v>
-      </c>
-      <c r="AE2">
-        <v>1.570000052</v>
-      </c>
-      <c r="AF2">
-        <v>11.761</v>
-      </c>
-      <c r="AG2">
-        <v>5.480228006</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
-        <v>0</v>
-      </c>
-      <c r="AV2">
-        <v>0</v>
-      </c>
-      <c r="AW2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>1</v>
-      </c>
-      <c r="BE2">
-        <v>0</v>
-      </c>
-      <c r="BF2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
+      <c r="G3">
+        <v>87.87672424</v>
+      </c>
+      <c r="H3">
+        <v>81.25119979</v>
+      </c>
+      <c r="I3">
+        <v>91.46945952999999</v>
+      </c>
+      <c r="J3">
+        <v>0.9334032370000001</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>17.28199959</v>
+      </c>
+      <c r="M3">
+        <v>4.796000004</v>
+      </c>
+      <c r="N3">
+        <v>68.65499878</v>
+      </c>
+      <c r="O3">
+        <v>6.922999859</v>
+      </c>
+      <c r="P3">
+        <v>24.42200089</v>
+      </c>
+      <c r="Q3">
+        <v>40.36113967</v>
+      </c>
+      <c r="R3">
+        <v>9.718943229000001</v>
+      </c>
+      <c r="S3">
+        <v>3310</v>
+      </c>
+      <c r="T3">
+        <v>1858121723</v>
+      </c>
+      <c r="U3">
+        <v>0.611212666</v>
+      </c>
+      <c r="V3">
+        <v>0.05</v>
+      </c>
+      <c r="W3">
+        <v>40.26</v>
+      </c>
+      <c r="X3">
+        <v>12.6</v>
+      </c>
+      <c r="Y3">
+        <v>86.8</v>
+      </c>
+      <c r="Z3">
+        <v>23</v>
+      </c>
+      <c r="AA3">
+        <v>42.09588617</v>
+      </c>
+      <c r="AB3">
+        <v>20.8</v>
+      </c>
+      <c r="AC3">
+        <v>25.3</v>
+      </c>
+      <c r="AD3">
+        <v>10.34799957</v>
+      </c>
+      <c r="AE3">
+        <v>64.84</v>
+      </c>
+      <c r="AF3">
+        <v>2.315808738</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>1</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>1</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
+      <c r="BF3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:59">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3">
-        <v>3310</v>
-      </c>
-      <c r="D3">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3">
-        <v>87.87672424</v>
-      </c>
-      <c r="J3">
-        <v>81.25119979</v>
-      </c>
-      <c r="K3">
-        <v>91.46945952999999</v>
-      </c>
-      <c r="L3">
-        <v>0.9334032370000001</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3">
-        <v>17.28199959</v>
-      </c>
-      <c r="O3">
-        <v>4.796000004</v>
-      </c>
-      <c r="P3">
-        <v>68.65499878</v>
-      </c>
-      <c r="Q3">
-        <v>6.922999859</v>
-      </c>
-      <c r="R3">
-        <v>24.42200089</v>
-      </c>
-      <c r="S3">
-        <v>40.36113967</v>
-      </c>
-      <c r="T3">
-        <v>9.718943229000001</v>
-      </c>
-      <c r="U3">
-        <v>1858121723</v>
-      </c>
-      <c r="V3">
-        <v>0.611212666</v>
-      </c>
-      <c r="W3">
-        <v>0.05</v>
-      </c>
-      <c r="X3">
-        <v>40.26</v>
-      </c>
-      <c r="Y3">
-        <v>12.6</v>
-      </c>
-      <c r="Z3">
-        <v>86.8</v>
-      </c>
-      <c r="AA3">
-        <v>23</v>
-      </c>
-      <c r="AB3">
-        <v>42.09588617</v>
-      </c>
-      <c r="AC3">
-        <v>20.8</v>
-      </c>
-      <c r="AD3">
-        <v>25.3</v>
-      </c>
-      <c r="AE3">
-        <v>10.34799957</v>
-      </c>
-      <c r="AF3">
-        <v>64.84</v>
-      </c>
-      <c r="AG3">
-        <v>2.315808738</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>1</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="AZ3">
-        <v>1</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
-      </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
-      <c r="BD3">
-        <v>1</v>
-      </c>
-      <c r="BE3">
-        <v>0</v>
-      </c>
-      <c r="BF3">
-        <v>0</v>
-      </c>
-      <c r="BG3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:58">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>60</v>
       </c>
-      <c r="C4">
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4">
+        <v>72.91772460999999</v>
+      </c>
+      <c r="H4">
+        <v>66.79169892</v>
+      </c>
+      <c r="I4">
+        <v>88.52062988</v>
+      </c>
+      <c r="J4">
+        <v>0.202814119</v>
+      </c>
+      <c r="K4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <v>18.89999962</v>
+      </c>
+      <c r="M4">
+        <v>9.661999701999999</v>
+      </c>
+      <c r="N4">
+        <v>54.98300171</v>
+      </c>
+      <c r="O4">
+        <v>15.57699966</v>
+      </c>
+      <c r="P4">
+        <v>29.44099998</v>
+      </c>
+      <c r="Q4">
+        <v>16.87471351</v>
+      </c>
+      <c r="R4">
+        <v>0.72227588</v>
+      </c>
+      <c r="S4">
         <v>830</v>
       </c>
-      <c r="D4">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4">
-        <v>72.91772460999999</v>
-      </c>
-      <c r="J4">
-        <v>66.79169892</v>
-      </c>
-      <c r="K4">
-        <v>88.52062988</v>
-      </c>
-      <c r="L4">
-        <v>0.202814119</v>
-      </c>
-      <c r="M4">
-        <v>6</v>
-      </c>
-      <c r="N4">
-        <v>18.89999962</v>
-      </c>
-      <c r="O4">
-        <v>9.661999701999999</v>
-      </c>
-      <c r="P4">
-        <v>54.98300171</v>
-      </c>
-      <c r="Q4">
-        <v>15.57699966</v>
-      </c>
-      <c r="R4">
-        <v>29.44099998</v>
-      </c>
-      <c r="S4">
-        <v>16.87471351</v>
-      </c>
       <c r="T4">
-        <v>0.72227588</v>
+        <v>647720707.1</v>
       </c>
       <c r="U4">
-        <v>647720707.1</v>
+        <v>2.061639469</v>
       </c>
       <c r="V4">
-        <v>2.061639469</v>
+        <v>0.01</v>
       </c>
       <c r="W4">
-        <v>0.01</v>
-      </c>
-      <c r="X4">
         <v>6.98</v>
       </c>
+      <c r="Y4">
+        <v>77.8</v>
+      </c>
       <c r="Z4">
-        <v>77.8</v>
+        <v>78.3</v>
       </c>
       <c r="AA4">
-        <v>78.3</v>
+        <v>17.11820358</v>
       </c>
       <c r="AB4">
-        <v>17.11820358</v>
+        <v>3</v>
       </c>
       <c r="AC4">
-        <v>3</v>
+        <v>22.6</v>
       </c>
       <c r="AD4">
-        <v>22.6</v>
+        <v>4.361999989</v>
       </c>
       <c r="AE4">
-        <v>4.361999989</v>
+        <v>28.193</v>
       </c>
       <c r="AF4">
-        <v>28.193</v>
+        <v>2.699437729</v>
       </c>
       <c r="AG4">
-        <v>2.699437729</v>
+        <v>0</v>
       </c>
       <c r="AH4">
         <v>0</v>
@@ -1327,13 +1315,13 @@
         <v>0</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY4">
         <v>1</v>
       </c>
       <c r="AZ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA4">
         <v>0</v>
@@ -1342,10 +1330,10 @@
         <v>0</v>
       </c>
       <c r="BC4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE4">
         <v>0</v>
@@ -1353,106 +1341,103 @@
       <c r="BF4">
         <v>0</v>
       </c>
-      <c r="BG4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:58">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="C5">
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5">
+        <v>13.5</v>
+      </c>
+      <c r="H5">
+        <v>0.4</v>
+      </c>
+      <c r="I5">
+        <v>42</v>
+      </c>
+      <c r="J5">
+        <v>0.06336919100000001</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>24.9109993</v>
+      </c>
+      <c r="M5">
+        <v>10.29500008</v>
+      </c>
+      <c r="N5">
+        <v>81.34899901999999</v>
+      </c>
+      <c r="O5">
+        <v>12.20400047</v>
+      </c>
+      <c r="P5">
+        <v>6.447000027</v>
+      </c>
+      <c r="Q5">
+        <v>36.83218885</v>
+      </c>
+      <c r="R5">
+        <v>5.131664248</v>
+      </c>
+      <c r="S5">
         <v>440</v>
       </c>
-      <c r="D5">
-        <v>45</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5">
-        <v>13.5</v>
-      </c>
-      <c r="J5">
-        <v>0.4</v>
-      </c>
-      <c r="K5">
-        <v>42</v>
-      </c>
-      <c r="L5">
-        <v>0.06336919100000001</v>
-      </c>
-      <c r="M5">
-        <v>6</v>
-      </c>
-      <c r="N5">
-        <v>24.9109993</v>
-      </c>
-      <c r="O5">
-        <v>10.29500008</v>
-      </c>
-      <c r="P5">
-        <v>81.34899901999999</v>
-      </c>
-      <c r="Q5">
-        <v>12.20400047</v>
-      </c>
-      <c r="R5">
-        <v>6.447000027</v>
-      </c>
-      <c r="S5">
-        <v>36.83218885</v>
-      </c>
       <c r="T5">
-        <v>5.131664248</v>
+        <v>35917650630</v>
       </c>
       <c r="U5">
-        <v>35917650630</v>
+        <v>9.470288097999999</v>
       </c>
       <c r="V5">
-        <v>9.470288097999999</v>
+        <v>0.03</v>
       </c>
       <c r="W5">
-        <v>0.03</v>
-      </c>
-      <c r="X5">
         <v>3</v>
       </c>
+      <c r="Y5">
+        <v>77</v>
+      </c>
       <c r="Z5">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="AA5">
-        <v>101</v>
+        <v>46.57451961</v>
       </c>
       <c r="AB5">
-        <v>46.57451961</v>
+        <v>10.6</v>
       </c>
       <c r="AC5">
-        <v>10.6</v>
+        <v>8</v>
       </c>
       <c r="AD5">
-        <v>8</v>
+        <v>3.707999945</v>
       </c>
       <c r="AE5">
-        <v>3.707999945</v>
+        <v>41.976</v>
       </c>
       <c r="AF5">
-        <v>41.976</v>
+        <v>4.553658283</v>
       </c>
       <c r="AG5">
-        <v>4.553658283</v>
+        <v>0</v>
       </c>
       <c r="AH5">
         <v>0</v>
@@ -1503,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="AX5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY5">
         <v>1</v>
       </c>
       <c r="AZ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA5">
         <v>0</v>
@@ -1518,10 +1503,10 @@
         <v>0</v>
       </c>
       <c r="BC5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE5">
         <v>0</v>
@@ -1529,106 +1514,103 @@
       <c r="BF5">
         <v>0</v>
       </c>
-      <c r="BG5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:58">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="C6">
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6">
+        <v>51.86239243</v>
+      </c>
+      <c r="H6">
+        <v>19.23297764</v>
+      </c>
+      <c r="I6">
+        <v>69.46530914</v>
+      </c>
+      <c r="J6">
+        <v>0.635369293</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>5.625</v>
+      </c>
+      <c r="M6">
+        <v>5.31799984</v>
+      </c>
+      <c r="N6">
+        <v>38.22900009</v>
+      </c>
+      <c r="O6">
+        <v>25</v>
+      </c>
+      <c r="P6">
+        <v>36.77099991</v>
+      </c>
+      <c r="Q6">
+        <v>72.98675034</v>
+      </c>
+      <c r="R6">
+        <v>20.36515297</v>
+      </c>
+      <c r="S6">
         <v>2520</v>
       </c>
-      <c r="D6">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6">
-        <v>51.86239243</v>
-      </c>
-      <c r="J6">
-        <v>19.23297764</v>
-      </c>
-      <c r="K6">
-        <v>69.46530914</v>
-      </c>
-      <c r="L6">
-        <v>0.635369293</v>
-      </c>
-      <c r="M6">
-        <v>10</v>
-      </c>
-      <c r="N6">
-        <v>5.625</v>
-      </c>
-      <c r="O6">
-        <v>5.31799984</v>
-      </c>
-      <c r="P6">
-        <v>38.22900009</v>
-      </c>
-      <c r="Q6">
-        <v>25</v>
-      </c>
-      <c r="R6">
-        <v>36.77099991</v>
-      </c>
-      <c r="S6">
-        <v>72.98675034</v>
-      </c>
       <c r="T6">
-        <v>20.36515297</v>
+        <v>14177437982</v>
       </c>
       <c r="U6">
-        <v>14177437982</v>
+        <v>6.779916158</v>
       </c>
       <c r="V6">
-        <v>6.779916158</v>
+        <v>0.29</v>
       </c>
       <c r="W6">
-        <v>0.29</v>
-      </c>
-      <c r="X6">
         <v>7.11</v>
       </c>
+      <c r="Y6">
+        <v>79.3</v>
+      </c>
       <c r="Z6">
-        <v>79.3</v>
+        <v>56.5</v>
       </c>
       <c r="AA6">
-        <v>56.5</v>
+        <v>53.17355571</v>
       </c>
       <c r="AB6">
-        <v>53.17355571</v>
+        <v>7.4</v>
       </c>
       <c r="AC6">
-        <v>7.4</v>
+        <v>32.3</v>
       </c>
       <c r="AD6">
-        <v>32.3</v>
+        <v>9.998000145000001</v>
       </c>
       <c r="AE6">
-        <v>9.998000145000001</v>
+        <v>64.95699999999999</v>
       </c>
       <c r="AF6">
-        <v>64.95699999999999</v>
+        <v>3.146204713</v>
       </c>
       <c r="AG6">
-        <v>3.146204713</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <v>0</v>
@@ -1679,13 +1661,13 @@
         <v>0</v>
       </c>
       <c r="AX6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY6">
         <v>1</v>
       </c>
       <c r="AZ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA6">
         <v>0</v>
@@ -1694,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="BC6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE6">
         <v>0</v>
@@ -1705,106 +1687,103 @@
       <c r="BF6">
         <v>0</v>
       </c>
-      <c r="BG6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:58">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>63</v>
       </c>
-      <c r="C7">
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7">
+        <v>61.9</v>
+      </c>
+      <c r="H7">
+        <v>36.54494476</v>
+      </c>
+      <c r="I7">
+        <v>83.9561824</v>
+      </c>
+      <c r="J7">
+        <v>0.490206046</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>18.99900055</v>
+      </c>
+      <c r="M7">
+        <v>8.211000443</v>
+      </c>
+      <c r="N7">
+        <v>50.375</v>
+      </c>
+      <c r="O7">
+        <v>5.986000061</v>
+      </c>
+      <c r="P7">
+        <v>43.63999939</v>
+      </c>
+      <c r="Q7">
+        <v>36.6588334</v>
+      </c>
+      <c r="R7">
+        <v>1.240430526</v>
+      </c>
+      <c r="S7">
         <v>1460</v>
       </c>
-      <c r="D7">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7">
-        <v>61.9</v>
-      </c>
-      <c r="J7">
-        <v>36.54494476</v>
-      </c>
-      <c r="K7">
-        <v>83.9561824</v>
-      </c>
-      <c r="L7">
-        <v>0.490206046</v>
-      </c>
-      <c r="M7">
-        <v>10</v>
-      </c>
-      <c r="N7">
-        <v>18.99900055</v>
-      </c>
-      <c r="O7">
-        <v>8.211000443</v>
-      </c>
-      <c r="P7">
-        <v>50.375</v>
-      </c>
-      <c r="Q7">
-        <v>5.986000061</v>
-      </c>
-      <c r="R7">
-        <v>43.63999939</v>
-      </c>
-      <c r="S7">
-        <v>36.6588334</v>
-      </c>
       <c r="T7">
-        <v>1.240430526</v>
+        <v>35372603446</v>
       </c>
       <c r="U7">
-        <v>35372603446</v>
+        <v>8.79407739</v>
       </c>
       <c r="V7">
-        <v>8.79407739</v>
+        <v>0.15</v>
       </c>
       <c r="W7">
-        <v>0.15</v>
-      </c>
-      <c r="X7">
         <v>19.2742298</v>
       </c>
+      <c r="Y7">
+        <v>43.90842056</v>
+      </c>
       <c r="Z7">
-        <v>43.90842056</v>
+        <v>98.3</v>
       </c>
       <c r="AA7">
-        <v>98.3</v>
+        <v>26.27654966</v>
       </c>
       <c r="AB7">
-        <v>26.27654966</v>
+        <v>9.4</v>
       </c>
       <c r="AC7">
-        <v>9.4</v>
+        <v>13.97364016</v>
       </c>
       <c r="AD7">
-        <v>13.97364016</v>
+        <v>2.747999907</v>
       </c>
       <c r="AE7">
-        <v>2.747999907</v>
+        <v>53.479</v>
       </c>
       <c r="AF7">
-        <v>53.479</v>
+        <v>3.881971936</v>
       </c>
       <c r="AG7">
-        <v>3.881971936</v>
+        <v>0</v>
       </c>
       <c r="AH7">
         <v>0</v>
@@ -1855,10 +1834,10 @@
         <v>0</v>
       </c>
       <c r="AX7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ7">
         <v>0</v>
@@ -1881,106 +1860,103 @@
       <c r="BF7">
         <v>0</v>
       </c>
-      <c r="BG7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:58">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>64</v>
       </c>
-      <c r="C8">
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8">
+        <v>67.05870819</v>
+      </c>
+      <c r="H8">
+        <v>51.01377073</v>
+      </c>
+      <c r="I8">
+        <v>91.37228394</v>
+      </c>
+      <c r="J8">
+        <v>4.733816529</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>16.01600075</v>
+      </c>
+      <c r="M8">
+        <v>5.980000019</v>
+      </c>
+      <c r="N8">
+        <v>54.96300125</v>
+      </c>
+      <c r="O8">
+        <v>8.237000464999999</v>
+      </c>
+      <c r="P8">
+        <v>36.79999924</v>
+      </c>
+      <c r="Q8">
+        <v>65.9632886</v>
+      </c>
+      <c r="R8">
+        <v>0.772319187</v>
+      </c>
+      <c r="S8">
         <v>13140</v>
       </c>
-      <c r="D8">
-        <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8">
-        <v>67.05870819</v>
-      </c>
-      <c r="J8">
-        <v>51.01377073</v>
-      </c>
-      <c r="K8">
-        <v>91.37228394</v>
-      </c>
-      <c r="L8">
-        <v>4.733816529</v>
-      </c>
-      <c r="M8">
-        <v>6</v>
-      </c>
-      <c r="N8">
-        <v>16.01600075</v>
-      </c>
-      <c r="O8">
-        <v>5.980000019</v>
-      </c>
-      <c r="P8">
-        <v>54.96300125</v>
-      </c>
-      <c r="Q8">
-        <v>8.237000464999999</v>
-      </c>
-      <c r="R8">
-        <v>36.79999924</v>
-      </c>
-      <c r="S8">
-        <v>65.9632886</v>
-      </c>
       <c r="T8">
-        <v>0.772319187</v>
+        <v>21736500713</v>
       </c>
       <c r="U8">
-        <v>21736500713</v>
+        <v>0.415061836</v>
       </c>
       <c r="V8">
-        <v>0.415061836</v>
+        <v>0.49</v>
       </c>
       <c r="W8">
-        <v>0.49</v>
-      </c>
-      <c r="X8">
         <v>18.86</v>
       </c>
+      <c r="Y8">
+        <v>95.3</v>
+      </c>
       <c r="Z8">
-        <v>95.3</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="AA8">
-        <v>97.09999999999999</v>
+        <v>46.69405811</v>
       </c>
       <c r="AB8">
-        <v>46.69405811</v>
+        <v>24</v>
       </c>
       <c r="AC8">
-        <v>24</v>
+        <v>8.298900808000001</v>
       </c>
       <c r="AD8">
-        <v>8.298900808000001</v>
+        <v>5.494999886</v>
       </c>
       <c r="AE8">
-        <v>5.494999886</v>
+        <v>39.756</v>
       </c>
       <c r="AF8">
-        <v>39.756</v>
+        <v>4.514037661</v>
       </c>
       <c r="AG8">
-        <v>4.514037661</v>
+        <v>0</v>
       </c>
       <c r="AH8">
         <v>0</v>
@@ -2031,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="AX8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY8">
         <v>1</v>
       </c>
       <c r="AZ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA8">
         <v>0</v>
@@ -2057,106 +2033,103 @@
       <c r="BF8">
         <v>0</v>
       </c>
-      <c r="BG8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:58">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="C9">
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9">
+        <v>78.3</v>
+      </c>
+      <c r="H9">
+        <v>63</v>
+      </c>
+      <c r="I9">
+        <v>90.8</v>
+      </c>
+      <c r="J9">
+        <v>0.536533378</v>
+      </c>
+      <c r="K9">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>27.77700043</v>
+      </c>
+      <c r="M9">
+        <v>15.79800034</v>
+      </c>
+      <c r="N9">
+        <v>44.72000122</v>
+      </c>
+      <c r="O9">
+        <v>14.10700035</v>
+      </c>
+      <c r="P9">
+        <v>41.17300034</v>
+      </c>
+      <c r="Q9">
+        <v>39.52355867</v>
+      </c>
+      <c r="R9">
+        <v>8.604962551</v>
+      </c>
+      <c r="S9">
         <v>1590</v>
       </c>
-      <c r="D9">
-        <v>74</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9">
-        <v>78.3</v>
-      </c>
-      <c r="J9">
-        <v>63</v>
-      </c>
-      <c r="K9">
-        <v>90.8</v>
-      </c>
-      <c r="L9">
-        <v>0.536533378</v>
-      </c>
-      <c r="M9">
-        <v>11</v>
-      </c>
-      <c r="N9">
-        <v>27.77700043</v>
-      </c>
-      <c r="O9">
-        <v>15.79800034</v>
-      </c>
-      <c r="P9">
-        <v>44.72000122</v>
-      </c>
-      <c r="Q9">
-        <v>14.10700035</v>
-      </c>
-      <c r="R9">
-        <v>41.17300034</v>
-      </c>
-      <c r="S9">
-        <v>39.52355867</v>
-      </c>
       <c r="T9">
-        <v>8.604962551</v>
+        <v>39086625009</v>
       </c>
       <c r="U9">
-        <v>39086625009</v>
+        <v>3.985865624</v>
       </c>
       <c r="V9">
-        <v>3.985865624</v>
+        <v>0.11</v>
       </c>
       <c r="W9">
-        <v>0.11</v>
-      </c>
-      <c r="X9">
         <v>25.51773743</v>
       </c>
+      <c r="Y9">
+        <v>76.59999999999999</v>
+      </c>
       <c r="Z9">
-        <v>76.59999999999999</v>
+        <v>63.4</v>
       </c>
       <c r="AA9">
-        <v>63.4</v>
+        <v>25.35736494</v>
       </c>
       <c r="AB9">
-        <v>25.35736494</v>
+        <v>10.9</v>
       </c>
       <c r="AC9">
-        <v>10.9</v>
+        <v>20.3</v>
       </c>
       <c r="AD9">
-        <v>20.3</v>
+        <v>2.164000034</v>
       </c>
       <c r="AE9">
-        <v>2.164000034</v>
+        <v>53.392</v>
       </c>
       <c r="AF9">
-        <v>53.392</v>
+        <v>3.550496942</v>
       </c>
       <c r="AG9">
-        <v>3.550496942</v>
+        <v>0</v>
       </c>
       <c r="AH9">
         <v>0</v>
@@ -2207,13 +2180,13 @@
         <v>0</v>
       </c>
       <c r="AX9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY9">
         <v>1</v>
       </c>
       <c r="AZ9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA9">
         <v>0</v>
@@ -2222,10 +2195,10 @@
         <v>0</v>
       </c>
       <c r="BC9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE9">
         <v>0</v>
@@ -2233,109 +2206,106 @@
       <c r="BF9">
         <v>0</v>
       </c>
-      <c r="BG9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:58">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="C10">
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10">
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <v>12.6</v>
+      </c>
+      <c r="I10">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.310415314</v>
+      </c>
+      <c r="K10">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>53.45399857</v>
+      </c>
+      <c r="M10">
+        <v>25.95800018</v>
+      </c>
+      <c r="N10">
+        <v>37.63899994</v>
+      </c>
+      <c r="O10">
+        <v>14.90200043</v>
+      </c>
+      <c r="P10">
+        <v>47.45899963</v>
+      </c>
+      <c r="Q10">
+        <v>18.29698092</v>
+      </c>
+      <c r="R10">
+        <v>1.335986481</v>
+      </c>
+      <c r="S10">
         <v>1260</v>
       </c>
-      <c r="D10">
-        <v>101</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10">
-        <v>36</v>
-      </c>
-      <c r="J10">
-        <v>12.6</v>
-      </c>
-      <c r="K10">
-        <v>68.40000000000001</v>
-      </c>
-      <c r="L10">
-        <v>0.310415314</v>
-      </c>
-      <c r="M10">
-        <v>12</v>
-      </c>
-      <c r="N10">
-        <v>53.45399857</v>
-      </c>
-      <c r="O10">
-        <v>25.95800018</v>
-      </c>
-      <c r="P10">
-        <v>37.63899994</v>
-      </c>
-      <c r="Q10">
-        <v>14.90200043</v>
-      </c>
-      <c r="R10">
-        <v>47.45899963</v>
-      </c>
-      <c r="S10">
-        <v>18.29698092</v>
-      </c>
       <c r="T10">
-        <v>1.335986481</v>
+        <v>61448046802</v>
       </c>
       <c r="U10">
-        <v>61448046802</v>
+        <v>5.357116778</v>
       </c>
       <c r="V10">
-        <v>5.357116778</v>
+        <v>0.3</v>
       </c>
       <c r="W10">
-        <v>0.3</v>
+        <v>16.5</v>
       </c>
       <c r="X10">
-        <v>16.5</v>
+        <v>5.9</v>
       </c>
       <c r="Y10">
-        <v>5.9</v>
+        <v>78.73303986000001</v>
       </c>
       <c r="Z10">
-        <v>78.73303986000001</v>
+        <v>53.5</v>
       </c>
       <c r="AA10">
-        <v>53.5</v>
+        <v>16.52198912</v>
       </c>
       <c r="AB10">
-        <v>16.52198912</v>
+        <v>19.1</v>
       </c>
       <c r="AC10">
-        <v>19.1</v>
+        <v>16.87697939</v>
       </c>
       <c r="AD10">
-        <v>16.87697939</v>
+        <v>11.66699982</v>
       </c>
       <c r="AE10">
-        <v>11.66699982</v>
+        <v>25.197</v>
       </c>
       <c r="AF10">
-        <v>25.197</v>
+        <v>4.304922007</v>
       </c>
       <c r="AG10">
-        <v>4.304922007</v>
+        <v>0</v>
       </c>
       <c r="AH10">
         <v>0</v>
@@ -2412,106 +2382,103 @@
       <c r="BF10">
         <v>0</v>
       </c>
-      <c r="BG10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:58">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>145</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>67</v>
       </c>
-      <c r="C11">
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11">
+        <v>56.37191391</v>
+      </c>
+      <c r="H11">
+        <v>31.67585522</v>
+      </c>
+      <c r="I11">
+        <v>84.2855835</v>
+      </c>
+      <c r="J11">
+        <v>0.545622113</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>12.18200016</v>
+      </c>
+      <c r="M11">
+        <v>9.477000237</v>
+      </c>
+      <c r="N11">
+        <v>36.77999878</v>
+      </c>
+      <c r="O11">
+        <v>12.06200027</v>
+      </c>
+      <c r="P11">
+        <v>51.1590004</v>
+      </c>
+      <c r="Q11">
+        <v>18.43512605</v>
+      </c>
+      <c r="R11">
+        <v>0.818201344</v>
+      </c>
+      <c r="S11">
         <v>2980</v>
       </c>
-      <c r="D11">
-        <v>145</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11">
-        <v>56.37191391</v>
-      </c>
-      <c r="J11">
-        <v>31.67585522</v>
-      </c>
-      <c r="K11">
-        <v>84.2855835</v>
-      </c>
-      <c r="L11">
-        <v>0.545622113</v>
-      </c>
-      <c r="M11">
-        <v>9</v>
-      </c>
-      <c r="N11">
-        <v>12.18200016</v>
-      </c>
-      <c r="O11">
-        <v>9.477000237</v>
-      </c>
-      <c r="P11">
-        <v>36.77999878</v>
-      </c>
-      <c r="Q11">
-        <v>12.06200027</v>
-      </c>
-      <c r="R11">
-        <v>51.1590004</v>
-      </c>
-      <c r="S11">
-        <v>18.43512605</v>
-      </c>
       <c r="T11">
-        <v>0.818201344</v>
+        <v>568499000000</v>
       </c>
       <c r="U11">
-        <v>568499000000</v>
+        <v>6.309718596</v>
       </c>
       <c r="V11">
-        <v>6.309718596</v>
+        <v>0.21</v>
       </c>
       <c r="W11">
-        <v>0.21</v>
-      </c>
-      <c r="X11">
         <v>21</v>
       </c>
+      <c r="Y11">
+        <v>59.6</v>
+      </c>
       <c r="Z11">
-        <v>59.6</v>
+        <v>111.6</v>
       </c>
       <c r="AA11">
-        <v>111.6</v>
+        <v>41.60273017</v>
       </c>
       <c r="AB11">
-        <v>41.60273017</v>
+        <v>6.7</v>
       </c>
       <c r="AC11">
-        <v>6.7</v>
+        <v>3.5</v>
       </c>
       <c r="AD11">
-        <v>3.5</v>
+        <v>4.559999943</v>
       </c>
       <c r="AE11">
-        <v>4.559999943</v>
+        <v>46.942</v>
       </c>
       <c r="AF11">
-        <v>46.942</v>
+        <v>4.48255153</v>
       </c>
       <c r="AG11">
-        <v>4.48255153</v>
+        <v>0</v>
       </c>
       <c r="AH11">
         <v>0</v>
@@ -2562,13 +2529,13 @@
         <v>0</v>
       </c>
       <c r="AX11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY11">
         <v>1</v>
       </c>
       <c r="AZ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA11">
         <v>0</v>
@@ -2577,10 +2544,10 @@
         <v>0</v>
       </c>
       <c r="BC11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE11">
         <v>0</v>
@@ -2588,106 +2555,103 @@
       <c r="BF11">
         <v>0</v>
       </c>
-      <c r="BG11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:58">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>162</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
         <v>68</v>
       </c>
-      <c r="C12">
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12">
+        <v>19.8</v>
+      </c>
+      <c r="H12">
+        <v>9.1</v>
+      </c>
+      <c r="I12">
+        <v>71.8</v>
+      </c>
+      <c r="J12">
+        <v>0.074016446</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>12.77900028</v>
+      </c>
+      <c r="M12">
+        <v>6.039000034</v>
+      </c>
+      <c r="N12">
+        <v>68.45300293</v>
+      </c>
+      <c r="O12">
+        <v>7.913000107</v>
+      </c>
+      <c r="P12">
+        <v>23.63400078</v>
+      </c>
+      <c r="Q12">
+        <v>14.72211453</v>
+      </c>
+      <c r="R12">
+        <v>3.926137464</v>
+      </c>
+      <c r="S12">
         <v>700</v>
       </c>
-      <c r="D12">
-        <v>162</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12">
-        <v>19.8</v>
-      </c>
-      <c r="J12">
-        <v>9.1</v>
-      </c>
-      <c r="K12">
-        <v>71.8</v>
-      </c>
-      <c r="L12">
-        <v>0.074016446</v>
-      </c>
-      <c r="M12">
-        <v>6</v>
-      </c>
-      <c r="N12">
-        <v>12.77900028</v>
-      </c>
-      <c r="O12">
-        <v>6.039000034</v>
-      </c>
-      <c r="P12">
-        <v>68.45300293</v>
-      </c>
-      <c r="Q12">
-        <v>7.913000107</v>
-      </c>
-      <c r="R12">
-        <v>23.63400078</v>
-      </c>
-      <c r="S12">
-        <v>14.72211453</v>
-      </c>
       <c r="T12">
-        <v>3.926137464</v>
+        <v>8016591928</v>
       </c>
       <c r="U12">
-        <v>8016591928</v>
+        <v>7.62457575</v>
       </c>
       <c r="V12">
-        <v>7.62457575</v>
+        <v>0.14</v>
       </c>
       <c r="W12">
-        <v>0.14</v>
-      </c>
-      <c r="X12">
         <v>10.6</v>
       </c>
+      <c r="Y12">
+        <v>70.5</v>
+      </c>
       <c r="Z12">
-        <v>70.5</v>
+        <v>43.4</v>
       </c>
       <c r="AA12">
-        <v>43.4</v>
+        <v>51.86310993</v>
       </c>
       <c r="AB12">
-        <v>51.86310993</v>
+        <v>63.8</v>
       </c>
       <c r="AC12">
-        <v>63.8</v>
+        <v>13.31802943</v>
       </c>
       <c r="AD12">
-        <v>13.31802943</v>
+        <v>1.169999957</v>
       </c>
       <c r="AE12">
-        <v>1.169999957</v>
+        <v>27.841</v>
       </c>
       <c r="AF12">
-        <v>27.841</v>
+        <v>6.054470586</v>
       </c>
       <c r="AG12">
-        <v>6.054470586</v>
+        <v>0</v>
       </c>
       <c r="AH12">
         <v>0</v>
@@ -2738,13 +2702,13 @@
         <v>0</v>
       </c>
       <c r="AX12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY12">
         <v>1</v>
       </c>
       <c r="AZ12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA12">
         <v>0</v>
@@ -2764,106 +2728,103 @@
       <c r="BF12">
         <v>0</v>
       </c>
-      <c r="BG12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:58">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>167</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>69</v>
       </c>
-      <c r="C13">
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13">
+        <v>61</v>
+      </c>
+      <c r="H13">
+        <v>32.7</v>
+      </c>
+      <c r="I13">
+        <v>85</v>
+      </c>
+      <c r="J13">
+        <v>0.608809117</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>16.31599998</v>
+      </c>
+      <c r="M13">
+        <v>5.46999979</v>
+      </c>
+      <c r="N13">
+        <v>53.67399979</v>
+      </c>
+      <c r="O13">
+        <v>20.20499992</v>
+      </c>
+      <c r="P13">
+        <v>26.12100029</v>
+      </c>
+      <c r="Q13">
+        <v>28.12071229</v>
+      </c>
+      <c r="R13">
+        <v>2.630373382</v>
+      </c>
+      <c r="S13">
         <v>1030</v>
       </c>
-      <c r="D13">
-        <v>167</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13">
-        <v>61</v>
-      </c>
-      <c r="J13">
-        <v>32.7</v>
-      </c>
-      <c r="K13">
-        <v>85</v>
-      </c>
-      <c r="L13">
-        <v>0.608809117</v>
-      </c>
-      <c r="M13">
-        <v>11</v>
-      </c>
-      <c r="N13">
-        <v>16.31599998</v>
-      </c>
-      <c r="O13">
-        <v>5.46999979</v>
-      </c>
-      <c r="P13">
-        <v>53.67399979</v>
-      </c>
-      <c r="Q13">
-        <v>20.20499992</v>
-      </c>
-      <c r="R13">
-        <v>26.12100029</v>
-      </c>
-      <c r="S13">
-        <v>28.12071229</v>
-      </c>
       <c r="T13">
-        <v>2.630373382</v>
+        <v>15304363138</v>
       </c>
       <c r="U13">
-        <v>15304363138</v>
+        <v>4.075083326</v>
       </c>
       <c r="V13">
-        <v>4.075083326</v>
+        <v>0.01</v>
       </c>
       <c r="W13">
-        <v>0.01</v>
-      </c>
-      <c r="X13">
         <v>17.7</v>
       </c>
+      <c r="Y13">
+        <v>57.7</v>
+      </c>
       <c r="Z13">
-        <v>57.7</v>
+        <v>52.3</v>
       </c>
       <c r="AA13">
-        <v>52.3</v>
+        <v>35.99474681</v>
       </c>
       <c r="AB13">
-        <v>35.99474681</v>
+        <v>43.3</v>
       </c>
       <c r="AC13">
-        <v>43.3</v>
+        <v>19.6238999</v>
       </c>
       <c r="AD13">
-        <v>19.6238999</v>
+        <v>6.356999874</v>
       </c>
       <c r="AE13">
-        <v>6.356999874</v>
+        <v>43.393</v>
       </c>
       <c r="AF13">
-        <v>43.393</v>
+        <v>3.697122779</v>
       </c>
       <c r="AG13">
-        <v>3.697122779</v>
+        <v>0</v>
       </c>
       <c r="AH13">
         <v>0</v>
@@ -2914,13 +2875,13 @@
         <v>0</v>
       </c>
       <c r="AX13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY13">
         <v>1</v>
       </c>
       <c r="AZ13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA13">
         <v>0</v>
@@ -2940,106 +2901,103 @@
       <c r="BF13">
         <v>0</v>
       </c>
-      <c r="BG13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:58">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="C14">
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14">
+        <v>44.9</v>
+      </c>
+      <c r="H14">
+        <v>31.7</v>
+      </c>
+      <c r="I14">
+        <v>76.3</v>
+      </c>
+      <c r="J14">
+        <v>0.299732598</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <v>26.11599922</v>
+      </c>
+      <c r="M14">
+        <v>9.135000228999999</v>
+      </c>
+      <c r="N14">
+        <v>53.35599899</v>
+      </c>
+      <c r="O14">
+        <v>18.83399963</v>
+      </c>
+      <c r="P14">
+        <v>27.80999947</v>
+      </c>
+      <c r="Q14">
+        <v>8.149134518</v>
+      </c>
+      <c r="R14">
+        <v>1.523136574</v>
+      </c>
+      <c r="S14">
         <v>1830</v>
       </c>
-      <c r="D14">
-        <v>185</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14">
-        <v>44.9</v>
-      </c>
-      <c r="J14">
-        <v>31.7</v>
-      </c>
-      <c r="K14">
-        <v>76.3</v>
-      </c>
-      <c r="L14">
-        <v>0.299732598</v>
-      </c>
-      <c r="M14">
-        <v>8</v>
-      </c>
-      <c r="N14">
-        <v>26.11599922</v>
-      </c>
-      <c r="O14">
-        <v>9.135000228999999</v>
-      </c>
-      <c r="P14">
-        <v>53.35599899</v>
-      </c>
-      <c r="Q14">
-        <v>18.83399963</v>
-      </c>
-      <c r="R14">
-        <v>27.80999947</v>
-      </c>
-      <c r="S14">
-        <v>8.149134518</v>
-      </c>
       <c r="T14">
-        <v>1.523136574</v>
+        <v>82151588419</v>
       </c>
       <c r="U14">
-        <v>82151588419</v>
+        <v>2.679411813</v>
       </c>
       <c r="V14">
-        <v>2.679411813</v>
+        <v>0.02</v>
       </c>
       <c r="W14">
-        <v>0.02</v>
-      </c>
-      <c r="X14">
         <v>24.64</v>
       </c>
+      <c r="Y14">
+        <v>75.90000000000001</v>
+      </c>
       <c r="Z14">
-        <v>75.90000000000001</v>
+        <v>69</v>
       </c>
       <c r="AA14">
-        <v>69</v>
+        <v>52.51987476</v>
       </c>
       <c r="AB14">
-        <v>52.51987476</v>
+        <v>24.3</v>
       </c>
       <c r="AC14">
-        <v>24.3</v>
+        <v>6.9</v>
       </c>
       <c r="AD14">
-        <v>6.9</v>
+        <v>12.74800014</v>
       </c>
       <c r="AE14">
-        <v>12.74800014</v>
+        <v>33.623</v>
       </c>
       <c r="AF14">
-        <v>33.623</v>
+        <v>2.867143272</v>
       </c>
       <c r="AG14">
-        <v>2.867143272</v>
+        <v>0</v>
       </c>
       <c r="AH14">
         <v>0</v>
@@ -3090,13 +3048,13 @@
         <v>0</v>
       </c>
       <c r="AX14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY14">
         <v>1</v>
       </c>
       <c r="AZ14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA14">
         <v>0</v>
@@ -3105,10 +3063,10 @@
         <v>0</v>
       </c>
       <c r="BC14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14">
         <v>0</v>
@@ -3116,109 +3074,106 @@
       <c r="BF14">
         <v>0</v>
       </c>
-      <c r="BG14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:58">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>203</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="C15">
-        <v>660</v>
-      </c>
-      <c r="D15">
-        <v>203</v>
-      </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
         <v>86</v>
       </c>
-      <c r="G15" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" t="s">
-        <v>87</v>
+      <c r="G15">
+        <v>20.4</v>
+      </c>
+      <c r="H15">
+        <v>10.3</v>
       </c>
       <c r="I15">
-        <v>20.4</v>
+        <v>51.4</v>
       </c>
       <c r="J15">
-        <v>10.3</v>
+        <v>0.134656001</v>
       </c>
       <c r="K15">
-        <v>51.4</v>
+        <v>7</v>
       </c>
       <c r="L15">
-        <v>0.134656001</v>
+        <v>19.75</v>
       </c>
       <c r="M15">
-        <v>7</v>
+        <v>12.92700005</v>
       </c>
       <c r="N15">
-        <v>19.75</v>
+        <v>71.54699707</v>
       </c>
       <c r="O15">
-        <v>12.92700005</v>
+        <v>6.887000084</v>
       </c>
       <c r="P15">
-        <v>71.54699707</v>
+        <v>21.56500053</v>
       </c>
       <c r="Q15">
-        <v>6.887000084</v>
+        <v>18.17025675</v>
       </c>
       <c r="R15">
-        <v>21.56500053</v>
+        <v>3.878679401</v>
       </c>
       <c r="S15">
-        <v>18.17025675</v>
+        <v>660</v>
       </c>
       <c r="T15">
-        <v>3.878679401</v>
+        <v>27291880327</v>
       </c>
       <c r="U15">
-        <v>27291880327</v>
+        <v>5.106307324</v>
       </c>
       <c r="V15">
-        <v>5.106307324</v>
+        <v>0.38</v>
       </c>
       <c r="W15">
-        <v>0.38</v>
+        <v>16.9</v>
       </c>
       <c r="X15">
-        <v>16.9</v>
+        <v>11.8</v>
       </c>
       <c r="Y15">
-        <v>11.8</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="Z15">
-        <v>78.40000000000001</v>
+        <v>60.1</v>
       </c>
       <c r="AA15">
-        <v>60.1</v>
+        <v>61.38641667</v>
       </c>
       <c r="AB15">
-        <v>61.38641667</v>
+        <v>35</v>
       </c>
       <c r="AC15">
-        <v>35</v>
+        <v>19.7</v>
       </c>
       <c r="AD15">
-        <v>19.7</v>
+        <v>1.907999992</v>
       </c>
       <c r="AE15">
-        <v>1.907999992</v>
+        <v>15.766</v>
       </c>
       <c r="AF15">
-        <v>15.766</v>
+        <v>5.459493493</v>
       </c>
       <c r="AG15">
-        <v>5.459493493</v>
+        <v>0</v>
       </c>
       <c r="AH15">
         <v>0</v>
@@ -3272,10 +3227,10 @@
         <v>0</v>
       </c>
       <c r="AY15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA15">
         <v>0</v>
@@ -3284,18 +3239,15 @@
         <v>0</v>
       </c>
       <c r="BC15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE15">
         <v>0</v>
       </c>
       <c r="BF15">
-        <v>0</v>
-      </c>
-      <c r="BG15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update init_data to fill NA in homicide rate with median
</commit_message>
<xml_diff>
--- a/output/clean_data.xlsx
+++ b/output/clean_data.xlsx
@@ -1552,6 +1552,9 @@
       <c r="W9">
         <v>25.51773743</v>
       </c>
+      <c r="X9">
+        <v>8.512840639152266</v>
+      </c>
       <c r="Y9">
         <v>76.59999999999999</v>
       </c>
@@ -2113,6 +2116,9 @@
       </c>
       <c r="W14">
         <v>24.64</v>
+      </c>
+      <c r="X14">
+        <v>8.512840639152266</v>
       </c>
       <c r="Y14">
         <v>75.90000000000001</v>

</xml_diff>